<commit_message>
Dodanie podstawowej ścieżki dźwiękowej lepszej niż disco polo
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Student\Desktop\game\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC95BC65-475B-4BFD-8125-6380F9FBCA67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="345" windowWidth="23040" windowHeight="12630" xr2:uid="{49F0EBDF-A5B3-4490-AA8C-8E415F793754}"/>
+    <workbookView xWindow="3930" yWindow="345" windowWidth="23040" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -144,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -471,11 +465,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Akcent 2" xfId="1" builtinId="33"/>
-    <cellStyle name="Akcent 3" xfId="2" builtinId="37"/>
-    <cellStyle name="Akcent 4" xfId="3" builtinId="41"/>
-    <cellStyle name="Akcent 6" xfId="4" builtinId="49"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Accent2" xfId="1" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="2" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="3" builtinId="41"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -849,18 +843,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2104DC3-A092-450F-9842-2ED575DC7EF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +863,7 @@
     <col min="4" max="4" width="69.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1150,7 +1145,7 @@
       </c>
       <c r="E24" s="25"/>
       <c r="F24" s="26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="3:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -1160,7 +1155,7 @@
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="3:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -1285,10 +1280,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I5" xr:uid="{A98A101C-7750-4B88-BC2C-F7A0B40E2485}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I5">
       <formula1>$F$4:$F$27</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F27" xr:uid="{D37B3B90-7106-4152-85C2-37C2F0ED4E56}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F27">
       <formula1>$I$3:$I$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>